<commit_message>
Further progress on the card object - next will be populating a few
</commit_message>
<xml_diff>
--- a/external/type_planning.xlsx
+++ b/external/type_planning.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Godot_Projects\fake_estate\external\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50E1D119-79DE-4451-9464-E14663A29F7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75816736-C8D9-4A96-A5D6-4EB95316649C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{F45CC606-5AA9-4BDD-8961-3562C5B64E95}"/>
+    <workbookView xWindow="39960" yWindow="1560" windowWidth="28800" windowHeight="15435" xr2:uid="{F45CC606-5AA9-4BDD-8961-3562C5B64E95}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="27">
   <si>
     <t>High Nerves</t>
   </si>
@@ -92,6 +92,30 @@
   </si>
   <si>
     <t>Just Happy To Be Here</t>
+  </si>
+  <si>
+    <t>`+ Nerves</t>
+  </si>
+  <si>
+    <t>`- Nerves</t>
+  </si>
+  <si>
+    <t>`+ Aggro</t>
+  </si>
+  <si>
+    <t>`+ Fatigue</t>
+  </si>
+  <si>
+    <t>`- Aggro</t>
+  </si>
+  <si>
+    <t>`- Fatigue</t>
+  </si>
+  <si>
+    <t>Speculate</t>
+  </si>
+  <si>
+    <t>Coax</t>
   </si>
 </sst>
 </file>
@@ -478,7 +502,7 @@
   <dimension ref="A1:P7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="P3" sqref="P3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -525,22 +549,22 @@
         <v>7</v>
       </c>
       <c r="K1" t="s">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="L1" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="M1" t="s">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="N1" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="O1" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="P1" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
@@ -562,7 +586,7 @@
         <v>16</v>
       </c>
       <c r="J2" t="s">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
@@ -586,10 +610,13 @@
         <v>15</v>
       </c>
       <c r="J3" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
+      <c r="O3" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
@@ -606,12 +633,15 @@
         <v>12</v>
       </c>
       <c r="J4" t="s">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="K4" s="4"/>
       <c r="L4" s="4"/>
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
+      <c r="O4" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
@@ -628,7 +658,7 @@
         <v>18</v>
       </c>
       <c r="J5" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="K5" s="4"/>
       <c r="L5" s="4"/>
@@ -646,7 +676,7 @@
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="J6" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="K6" s="4"/>
       <c r="L6" s="4"/>
@@ -666,7 +696,7 @@
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="J7" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="K7" s="4"/>
       <c r="L7" s="4"/>

</xml_diff>

<commit_message>
Haven't committed in some time, oops
</commit_message>
<xml_diff>
--- a/external/type_planning.xlsx
+++ b/external/type_planning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Godot_Projects\fake_estate\external\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75816736-C8D9-4A96-A5D6-4EB95316649C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1BC4BAF-FB20-47EA-B97F-A1ED631F3D8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="39960" yWindow="1560" windowWidth="28800" windowHeight="15435" xr2:uid="{F45CC606-5AA9-4BDD-8961-3562C5B64E95}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="34">
   <si>
     <t>High Nerves</t>
   </si>
@@ -116,6 +116,27 @@
   </si>
   <si>
     <t>Coax</t>
+  </si>
+  <si>
+    <t>Excite</t>
+  </si>
+  <si>
+    <t>Other cards</t>
+  </si>
+  <si>
+    <t>Force</t>
+  </si>
+  <si>
+    <t>Force a bid</t>
+  </si>
+  <si>
+    <t>Skip</t>
+  </si>
+  <si>
+    <t>Skip a bid</t>
+  </si>
+  <si>
+    <t>Reduce fatigure</t>
   </si>
 </sst>
 </file>
@@ -499,10 +520,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A8E636F-1774-498C-8B8B-E121AE023341}">
-  <dimension ref="A1:P7"/>
+  <dimension ref="A1:P12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P3" sqref="P3"/>
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -590,6 +611,9 @@
       </c>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
+      <c r="P2" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
@@ -705,6 +729,30 @@
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
     </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J11" t="s">
+        <v>29</v>
+      </c>
+      <c r="K11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J12" t="s">
+        <v>31</v>
+      </c>
+      <c r="K12" t="s">
+        <v>32</v>
+      </c>
+      <c r="L12" t="s">
+        <v>33</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>